<commit_message>
Customer portal Register TC commited
</commit_message>
<xml_diff>
--- a/src/test/resources/TestData.xlsx
+++ b/src/test/resources/TestData.xlsx
@@ -3,21 +3,21 @@
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
   <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="20415"/>
   <workbookPr defaultThemeVersion="166925"/>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:801_{168CF97A-4374-4569-ADBE-553C7898D5A7}" xr6:coauthVersionLast="36" xr6:coauthVersionMax="36" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:801_{81F50165-4838-4B6E-9C71-CB750A564DA8}" xr6:coauthVersionLast="36" xr6:coauthVersionMax="36" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="0" yWindow="0" windowWidth="12450" windowHeight="4170" activeTab="1" xr2:uid="{37B91979-A2CD-4275-8B46-28CAE73357A2}"/>
+    <workbookView xWindow="0" yWindow="0" windowWidth="13245" windowHeight="6015" activeTab="1" xr2:uid="{37B91979-A2CD-4275-8B46-28CAE73357A2}"/>
   </bookViews>
   <sheets>
-    <sheet name="TimeSheetModule" sheetId="3" r:id="rId1"/>
-    <sheet name="Timesheet_CancelRequests" sheetId="8" r:id="rId2"/>
+    <sheet name="KSIDC_CP_Login" sheetId="3" r:id="rId1"/>
+    <sheet name="KSIDC_Registration" sheetId="8" r:id="rId2"/>
     <sheet name="Timesheet_Approvals" sheetId="9" r:id="rId3"/>
     <sheet name="TimeSheeEditDelete" sheetId="4" r:id="rId4"/>
     <sheet name="TimesheetOnBehalf" sheetId="6" r:id="rId5"/>
     <sheet name="LeaveRequest" sheetId="5" r:id="rId6"/>
-    <sheet name="KSIDC_CP_Login" sheetId="7" r:id="rId7"/>
+    <sheet name="EWCLeaveRequest" sheetId="7" r:id="rId7"/>
   </sheets>
-  <calcPr calcId="191029"/>
-  <oleSize ref="B1:F11"/>
+  <calcPr calcId="0"/>
+  <oleSize ref="B1:G18"/>
   <extLst>
     <ext xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" uri="{140A7094-0E35-4892-8432-C4D2E57EDEB5}">
       <x15:workbookPr chartTrackingRefBase="1"/>
@@ -27,7 +27,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="150" uniqueCount="84">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="149" uniqueCount="95">
   <si>
     <t>Run</t>
   </si>
@@ -209,6 +209,9 @@
     <t xml:space="preserve"> Oracle America INC </t>
   </si>
   <si>
+    <t>TC_EWCLeaveRequestModule</t>
+  </si>
+  <si>
     <t>EWCType</t>
   </si>
   <si>
@@ -257,9 +260,6 @@
     <t>Extra Spare Day</t>
   </si>
   <si>
-    <t>TC_O360_TimesheetCancelRequests</t>
-  </si>
-  <si>
     <t xml:space="preserve"> Design/Development </t>
   </si>
   <si>
@@ -278,14 +278,47 @@
     <t>ProjectName2</t>
   </si>
   <si>
-    <t>TC_KSIDC_CP_Login</t>
+    <t>MobileNumber</t>
+  </si>
+  <si>
+    <t>VerificationCode</t>
+  </si>
+  <si>
+    <t>EmailAddress</t>
+  </si>
+  <si>
+    <t>ChiefPromoterFullName</t>
+  </si>
+  <si>
+    <t>CompanyPAN</t>
+  </si>
+  <si>
+    <t>Password</t>
+  </si>
+  <si>
+    <t>ConfirmPassword</t>
+  </si>
+  <si>
+    <t>Register_Page_Module</t>
+  </si>
+  <si>
+    <t>KSIDC.15@gmail.com</t>
+  </si>
+  <si>
+    <t>ABC54R34easew4</t>
+  </si>
+  <si>
+    <t>Ijgst6566y</t>
+  </si>
+  <si>
+    <t>KSIDCcp@123#</t>
   </si>
 </sst>
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="x14ac x16r2 xr">
-  <fonts count="3" x14ac:knownFonts="1">
+  <fonts count="4" x14ac:knownFonts="1">
     <font>
       <sz val="11"/>
       <color theme="1"/>
@@ -306,6 +339,14 @@
       <color rgb="FF1F1F1F"/>
       <name val="Consolas"/>
       <family val="3"/>
+    </font>
+    <font>
+      <u/>
+      <sz val="11"/>
+      <color theme="10"/>
+      <name val="Calibri"/>
+      <family val="2"/>
+      <scheme val="minor"/>
     </font>
   </fonts>
   <fills count="3">
@@ -357,10 +398,11 @@
       <diagonal/>
     </border>
   </borders>
-  <cellStyleXfs count="1">
+  <cellStyleXfs count="2">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
   </cellStyleXfs>
-  <cellXfs count="20">
+  <cellXfs count="24">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="1" fillId="2" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="1" xfId="0" applyBorder="1" applyAlignment="1">
@@ -401,8 +443,21 @@
     <xf numFmtId="0" fontId="1" fillId="2" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="1" xfId="0" applyBorder="1" applyAlignment="1"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="1" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1"/>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="1" xfId="1" quotePrefix="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="top" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="1" xfId="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="top" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="1" xfId="1" applyBorder="1" applyAlignment="1">
+      <alignment vertical="top" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
+      <alignment vertical="top" wrapText="1"/>
+    </xf>
   </cellXfs>
-  <cellStyles count="1">
+  <cellStyles count="2">
+    <cellStyle name="Hyperlink" xfId="1" builtinId="8"/>
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
   </cellStyles>
   <dxfs count="0"/>
@@ -718,7 +773,7 @@
   <dimension ref="A1:AN2"/>
   <sheetViews>
     <sheetView workbookViewId="0">
-      <selection activeCell="C7" sqref="C7"/>
+      <selection activeCell="C12" sqref="C12"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -802,10 +857,10 @@
         <v>58</v>
       </c>
       <c r="S1" s="17" t="s">
-        <v>73</v>
+        <v>74</v>
       </c>
       <c r="T1" s="17" t="s">
-        <v>74</v>
+        <v>75</v>
       </c>
       <c r="U1" s="1" t="s">
         <v>82</v>
@@ -874,10 +929,10 @@
         <v>27</v>
       </c>
       <c r="O2" s="2" t="s">
+        <v>73</v>
+      </c>
+      <c r="P2" s="11" t="s">
         <v>72</v>
-      </c>
-      <c r="P2" s="11" t="s">
-        <v>71</v>
       </c>
       <c r="Q2" s="3">
         <v>1</v>
@@ -919,10 +974,10 @@
 
 <file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{79F5BEBC-63DB-4F03-9AF6-8CE69341974D}">
-  <dimension ref="A1:I2"/>
+  <dimension ref="A1:S2"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="A2" sqref="A2"/>
+    <sheetView tabSelected="1" topLeftCell="B1" workbookViewId="0">
+      <selection activeCell="E9" sqref="E9"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -938,63 +993,88 @@
     <col min="9" max="9" width="27.85546875" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:9" x14ac:dyDescent="0.25">
-      <c r="A1" s="17" t="s">
+    <row r="1" spans="1:19" customFormat="1" x14ac:dyDescent="0.25">
+      <c r="A1" s="1" t="s">
+        <v>0</v>
+      </c>
+      <c r="B1" s="1" t="s">
         <v>1</v>
       </c>
-      <c r="B1" s="17" t="s">
-        <v>0</v>
-      </c>
-      <c r="C1" s="17" t="s">
-        <v>45</v>
-      </c>
-      <c r="D1" s="17" t="s">
-        <v>46</v>
-      </c>
-      <c r="E1" s="17" t="s">
-        <v>24</v>
-      </c>
-      <c r="F1" s="17" t="s">
-        <v>73</v>
-      </c>
-      <c r="G1" s="17" t="s">
-        <v>74</v>
-      </c>
-      <c r="H1" s="17" t="s">
-        <v>75</v>
+      <c r="C1" s="1" t="s">
+        <v>83</v>
+      </c>
+      <c r="D1" s="1" t="s">
+        <v>84</v>
+      </c>
+      <c r="E1" s="1" t="s">
+        <v>85</v>
+      </c>
+      <c r="F1" s="1" t="s">
+        <v>86</v>
+      </c>
+      <c r="G1" s="1" t="s">
+        <v>87</v>
+      </c>
+      <c r="H1" s="1" t="s">
+        <v>88</v>
       </c>
       <c r="I1" s="1" t="s">
-        <v>44</v>
-      </c>
+        <v>89</v>
+      </c>
+      <c r="J1" s="1"/>
+      <c r="K1" s="1"/>
+      <c r="L1" s="1"/>
+      <c r="M1" s="1"/>
+      <c r="N1" s="1"/>
+      <c r="O1" s="1"/>
+      <c r="P1" s="1"/>
+      <c r="Q1" s="1"/>
+      <c r="R1" s="1"/>
+      <c r="S1" s="1"/>
     </row>
-    <row r="2" spans="1:9" x14ac:dyDescent="0.25">
-      <c r="A2" s="18" t="s">
-        <v>76</v>
-      </c>
-      <c r="B2" s="18" t="s">
+    <row r="2" spans="1:19" s="23" customFormat="1" ht="30" x14ac:dyDescent="0.25">
+      <c r="A2" s="2" t="s">
         <v>2</v>
       </c>
-      <c r="C2" s="18" t="s">
-        <v>14</v>
-      </c>
-      <c r="D2" s="18" t="s">
-        <v>77</v>
-      </c>
-      <c r="E2" s="18" t="s">
-        <v>25</v>
-      </c>
-      <c r="F2" s="18" t="s">
-        <v>78</v>
-      </c>
-      <c r="G2" s="18" t="s">
-        <v>79</v>
-      </c>
-      <c r="H2" s="18"/>
-      <c r="I2" s="19" t="s">
-        <v>66</v>
-      </c>
+      <c r="B2" s="2" t="s">
+        <v>90</v>
+      </c>
+      <c r="C2" s="11">
+        <v>9954327855</v>
+      </c>
+      <c r="D2" s="5"/>
+      <c r="E2" s="20" t="s">
+        <v>91</v>
+      </c>
+      <c r="F2" s="20" t="s">
+        <v>92</v>
+      </c>
+      <c r="G2" s="4" t="s">
+        <v>93</v>
+      </c>
+      <c r="H2" s="21" t="s">
+        <v>94</v>
+      </c>
+      <c r="I2" s="22" t="s">
+        <v>94</v>
+      </c>
+      <c r="J2" s="2"/>
+      <c r="K2" s="2"/>
+      <c r="L2" s="2"/>
+      <c r="M2" s="5"/>
+      <c r="N2" s="3"/>
+      <c r="O2" s="2"/>
+      <c r="P2" s="2"/>
+      <c r="Q2" s="2"/>
+      <c r="R2" s="2"/>
+      <c r="S2" s="3"/>
     </row>
   </sheetData>
+  <hyperlinks>
+    <hyperlink ref="E2" r:id="rId1" display="shrilesha@gmail.com" xr:uid="{E10CFA88-92E5-4100-B1BD-DE75719F19BA}"/>
+    <hyperlink ref="H2" r:id="rId2" xr:uid="{CAD91A24-1147-4A9B-874E-5657A1369CBC}"/>
+    <hyperlink ref="I2" r:id="rId3" xr:uid="{DFE939FD-4140-437C-8DE2-DC8771EDCBA8}"/>
+  </hyperlinks>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
 </worksheet>
 </file>
@@ -1029,13 +1109,13 @@
         <v>24</v>
       </c>
       <c r="F1" s="17" t="s">
-        <v>73</v>
+        <v>74</v>
       </c>
       <c r="G1" s="17" t="s">
-        <v>74</v>
+        <v>75</v>
       </c>
       <c r="H1" s="17" t="s">
-        <v>75</v>
+        <v>76</v>
       </c>
       <c r="I1" s="1" t="s">
         <v>44</v>
@@ -1065,7 +1145,7 @@
       </c>
       <c r="H2" s="18"/>
       <c r="I2" s="19" t="s">
-        <v>66</v>
+        <v>67</v>
       </c>
     </row>
   </sheetData>
@@ -1449,7 +1529,7 @@
   <dimension ref="A1:AR3"/>
   <sheetViews>
     <sheetView workbookViewId="0">
-      <selection activeCell="C11" sqref="C11"/>
+      <selection activeCell="M3" sqref="M3"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -1475,7 +1555,7 @@
         <v>0</v>
       </c>
       <c r="C1" s="1" t="s">
-        <v>60</v>
+        <v>61</v>
       </c>
       <c r="D1" s="1" t="s">
         <v>33</v>
@@ -1505,13 +1585,13 @@
         <v>56</v>
       </c>
       <c r="M1" s="1" t="s">
-        <v>65</v>
+        <v>66</v>
       </c>
       <c r="N1" s="1" t="s">
-        <v>67</v>
+        <v>68</v>
       </c>
       <c r="O1" s="1" t="s">
-        <v>69</v>
+        <v>70</v>
       </c>
       <c r="P1" s="1"/>
       <c r="Q1" s="1"/>
@@ -1545,19 +1625,19 @@
     </row>
     <row r="2" spans="1:44" s="8" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A2" s="2" t="s">
-        <v>83</v>
+        <v>60</v>
       </c>
       <c r="B2" s="7" t="s">
         <v>2</v>
       </c>
       <c r="C2" s="2" t="s">
-        <v>62</v>
+        <v>63</v>
       </c>
       <c r="D2" s="3">
         <v>2024</v>
       </c>
       <c r="E2" s="3" t="s">
-        <v>63</v>
+        <v>64</v>
       </c>
       <c r="F2" s="12">
         <v>13</v>
@@ -1566,7 +1646,7 @@
         <v>2024</v>
       </c>
       <c r="H2" s="3" t="s">
-        <v>63</v>
+        <v>64</v>
       </c>
       <c r="I2" s="12">
         <v>15</v>
@@ -1575,19 +1655,19 @@
         <v>14</v>
       </c>
       <c r="K2" s="3" t="s">
-        <v>64</v>
+        <v>65</v>
       </c>
       <c r="L2" s="8" t="s">
         <v>51</v>
       </c>
       <c r="M2" s="3" t="s">
-        <v>66</v>
+        <v>67</v>
       </c>
       <c r="N2" s="2" t="s">
-        <v>68</v>
+        <v>69</v>
       </c>
       <c r="O2" s="8" t="s">
-        <v>70</v>
+        <v>71</v>
       </c>
       <c r="P2" s="3"/>
       <c r="Q2" s="2"/>
@@ -1619,7 +1699,7 @@
     </row>
     <row r="3" spans="1:44" x14ac:dyDescent="0.25">
       <c r="C3" s="2" t="s">
-        <v>61</v>
+        <v>62</v>
       </c>
     </row>
   </sheetData>

</xml_diff>

<commit_message>
Business information changes committed
</commit_message>
<xml_diff>
--- a/src/test/resources/TestData.xlsx
+++ b/src/test/resources/TestData.xlsx
@@ -3,21 +3,21 @@
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
   <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="20415"/>
   <workbookPr defaultThemeVersion="166925"/>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:801_{81F50165-4838-4B6E-9C71-CB750A564DA8}" xr6:coauthVersionLast="36" xr6:coauthVersionMax="36" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:801_{45BD66A4-6914-48E6-9411-7B0B3DCDB353}" xr6:coauthVersionLast="36" xr6:coauthVersionMax="36" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="0" yWindow="0" windowWidth="13245" windowHeight="6015" activeTab="1" xr2:uid="{37B91979-A2CD-4275-8B46-28CAE73357A2}"/>
+    <workbookView xWindow="0" yWindow="0" windowWidth="11925" windowHeight="6015" firstSheet="2" activeTab="2" xr2:uid="{37B91979-A2CD-4275-8B46-28CAE73357A2}"/>
   </bookViews>
   <sheets>
     <sheet name="KSIDC_CP_Login" sheetId="3" r:id="rId1"/>
     <sheet name="KSIDC_Registration" sheetId="8" r:id="rId2"/>
-    <sheet name="Timesheet_Approvals" sheetId="9" r:id="rId3"/>
+    <sheet name="KSIDC_Business_Information" sheetId="9" r:id="rId3"/>
     <sheet name="TimeSheeEditDelete" sheetId="4" r:id="rId4"/>
     <sheet name="TimesheetOnBehalf" sheetId="6" r:id="rId5"/>
     <sheet name="LeaveRequest" sheetId="5" r:id="rId6"/>
     <sheet name="EWCLeaveRequest" sheetId="7" r:id="rId7"/>
   </sheets>
   <calcPr calcId="0"/>
-  <oleSize ref="B1:G18"/>
+  <oleSize ref="A4:D21"/>
   <extLst>
     <ext xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" uri="{140A7094-0E35-4892-8432-C4D2E57EDEB5}">
       <x15:workbookPr chartTrackingRefBase="1"/>
@@ -27,7 +27,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="149" uniqueCount="95">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="160" uniqueCount="112">
   <si>
     <t>Run</t>
   </si>
@@ -257,21 +257,12 @@
     <t>New Day</t>
   </si>
   <si>
-    <t>Extra Spare Day</t>
-  </si>
-  <si>
-    <t xml:space="preserve"> Design/Development </t>
-  </si>
-  <si>
     <t>MON</t>
   </si>
   <si>
     <t>Tuesday</t>
   </si>
   <si>
-    <t>TC_O360_TimesheetApprovals</t>
-  </si>
-  <si>
     <t>Swiss solutions inc</t>
   </si>
   <si>
@@ -312,6 +303,66 @@
   </si>
   <si>
     <t>KSIDCcp@123#</t>
+  </si>
+  <si>
+    <t>DisplayName</t>
+  </si>
+  <si>
+    <t>DocketAmount</t>
+  </si>
+  <si>
+    <t>LoanAmountRequired</t>
+  </si>
+  <si>
+    <t>ProductServiceName</t>
+  </si>
+  <si>
+    <t>BreakEvenPeriod</t>
+  </si>
+  <si>
+    <t>ProjectImplementationPeriodInMonths</t>
+  </si>
+  <si>
+    <t>ApproxTotalLabourCount</t>
+  </si>
+  <si>
+    <t>DocketNumber</t>
+  </si>
+  <si>
+    <t>TreasuryReleaseDate</t>
+  </si>
+  <si>
+    <t>ProductionCapacityQuantityPerAnnumTest</t>
+  </si>
+  <si>
+    <t>Business_Information_Module</t>
+  </si>
+  <si>
+    <t>KSIDC_CP</t>
+  </si>
+  <si>
+    <t>5,00,00,000.00</t>
+  </si>
+  <si>
+    <t>1,00,00,000.00</t>
+  </si>
+  <si>
+    <t>GFDYR676</t>
+  </si>
+  <si>
+    <t>24</t>
+  </si>
+  <si>
+    <t>1000</t>
+  </si>
+  <si>
+    <t>HFIIK38743874</t>
+  </si>
+  <si>
+    <t>11/11/2024</t>
+  </si>
+  <si>
+    <t>DWE34DF33333</t>
   </si>
 </sst>
 </file>
@@ -402,7 +453,7 @@
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
     <xf numFmtId="0" fontId="3" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
   </cellStyleXfs>
-  <cellXfs count="24">
+  <cellXfs count="25">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="1" fillId="2" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="1" xfId="0" applyBorder="1" applyAlignment="1">
@@ -441,8 +492,6 @@
     <xf numFmtId="0" fontId="0" fillId="0" borderId="1" xfId="0" applyFill="1" applyBorder="1"/>
     <xf numFmtId="0" fontId="2" fillId="0" borderId="0" xfId="0" applyFont="1"/>
     <xf numFmtId="0" fontId="1" fillId="2" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1"/>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="1" xfId="0" applyBorder="1" applyAlignment="1"/>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="1" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1"/>
     <xf numFmtId="0" fontId="3" fillId="0" borderId="1" xfId="1" quotePrefix="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="left" vertical="top" wrapText="1"/>
     </xf>
@@ -455,6 +504,9 @@
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
       <alignment vertical="top" wrapText="1"/>
     </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" quotePrefix="1"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" quotePrefix="1" applyFill="1"/>
+    <xf numFmtId="14" fontId="0" fillId="0" borderId="0" xfId="0" quotePrefix="1" applyNumberFormat="1"/>
   </cellXfs>
   <cellStyles count="2">
     <cellStyle name="Hyperlink" xfId="1" builtinId="8"/>
@@ -863,7 +915,7 @@
         <v>75</v>
       </c>
       <c r="U1" s="1" t="s">
-        <v>82</v>
+        <v>79</v>
       </c>
       <c r="V1" s="1"/>
       <c r="W1" s="1"/>
@@ -941,13 +993,13 @@
         <v>59</v>
       </c>
       <c r="S2" s="7" t="s">
+        <v>76</v>
+      </c>
+      <c r="T2" s="7" t="s">
+        <v>77</v>
+      </c>
+      <c r="U2" s="3" t="s">
         <v>78</v>
-      </c>
-      <c r="T2" s="7" t="s">
-        <v>79</v>
-      </c>
-      <c r="U2" s="3" t="s">
-        <v>81</v>
       </c>
       <c r="V2" s="10"/>
       <c r="W2" s="10"/>
@@ -976,7 +1028,7 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{79F5BEBC-63DB-4F03-9AF6-8CE69341974D}">
   <dimension ref="A1:S2"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="B1" workbookViewId="0">
+    <sheetView topLeftCell="B1" workbookViewId="0">
       <selection activeCell="E9" sqref="E9"/>
     </sheetView>
   </sheetViews>
@@ -1001,25 +1053,25 @@
         <v>1</v>
       </c>
       <c r="C1" s="1" t="s">
+        <v>80</v>
+      </c>
+      <c r="D1" s="1" t="s">
+        <v>81</v>
+      </c>
+      <c r="E1" s="1" t="s">
+        <v>82</v>
+      </c>
+      <c r="F1" s="1" t="s">
         <v>83</v>
       </c>
-      <c r="D1" s="1" t="s">
+      <c r="G1" s="1" t="s">
         <v>84</v>
       </c>
-      <c r="E1" s="1" t="s">
+      <c r="H1" s="1" t="s">
         <v>85</v>
       </c>
-      <c r="F1" s="1" t="s">
+      <c r="I1" s="1" t="s">
         <v>86</v>
-      </c>
-      <c r="G1" s="1" t="s">
-        <v>87</v>
-      </c>
-      <c r="H1" s="1" t="s">
-        <v>88</v>
-      </c>
-      <c r="I1" s="1" t="s">
-        <v>89</v>
       </c>
       <c r="J1" s="1"/>
       <c r="K1" s="1"/>
@@ -1032,31 +1084,31 @@
       <c r="R1" s="1"/>
       <c r="S1" s="1"/>
     </row>
-    <row r="2" spans="1:19" s="23" customFormat="1" ht="30" x14ac:dyDescent="0.25">
+    <row r="2" spans="1:19" s="21" customFormat="1" ht="30" x14ac:dyDescent="0.25">
       <c r="A2" s="2" t="s">
         <v>2</v>
       </c>
       <c r="B2" s="2" t="s">
-        <v>90</v>
+        <v>87</v>
       </c>
       <c r="C2" s="11">
         <v>9954327855</v>
       </c>
       <c r="D2" s="5"/>
-      <c r="E2" s="20" t="s">
+      <c r="E2" s="18" t="s">
+        <v>88</v>
+      </c>
+      <c r="F2" s="18" t="s">
+        <v>89</v>
+      </c>
+      <c r="G2" s="4" t="s">
+        <v>90</v>
+      </c>
+      <c r="H2" s="19" t="s">
         <v>91</v>
       </c>
-      <c r="F2" s="20" t="s">
-        <v>92</v>
-      </c>
-      <c r="G2" s="4" t="s">
-        <v>93</v>
-      </c>
-      <c r="H2" s="21" t="s">
-        <v>94</v>
-      </c>
-      <c r="I2" s="22" t="s">
-        <v>94</v>
+      <c r="I2" s="20" t="s">
+        <v>91</v>
       </c>
       <c r="J2" s="2"/>
       <c r="K2" s="2"/>
@@ -1081,10 +1133,10 @@
 
 <file path=xl/worksheets/sheet3.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{E52F80EF-30F9-4CBE-97A9-F5DB22DCED8A}">
-  <dimension ref="A1:I2"/>
+  <dimension ref="A1:S2"/>
   <sheetViews>
-    <sheetView topLeftCell="A4" workbookViewId="0">
-      <selection activeCell="B1" sqref="B1"/>
+    <sheetView tabSelected="1" topLeftCell="A4" workbookViewId="0">
+      <selection activeCell="A10" sqref="A10"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="21.28515625" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -1092,60 +1144,97 @@
     <col min="1" max="1" width="32.140625" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:9" x14ac:dyDescent="0.25">
-      <c r="A1" s="17" t="s">
+    <row r="1" spans="1:19" customFormat="1" x14ac:dyDescent="0.25">
+      <c r="A1" s="1" t="s">
+        <v>0</v>
+      </c>
+      <c r="B1" s="1" t="s">
         <v>1</v>
       </c>
-      <c r="B1" s="17" t="s">
-        <v>0</v>
-      </c>
-      <c r="C1" s="17" t="s">
-        <v>45</v>
-      </c>
-      <c r="D1" s="17" t="s">
-        <v>46</v>
-      </c>
-      <c r="E1" s="17" t="s">
-        <v>24</v>
-      </c>
-      <c r="F1" s="17" t="s">
-        <v>74</v>
-      </c>
-      <c r="G1" s="17" t="s">
-        <v>75</v>
-      </c>
-      <c r="H1" s="17" t="s">
-        <v>76</v>
+      <c r="C1" s="1" t="s">
+        <v>82</v>
+      </c>
+      <c r="D1" s="1" t="s">
+        <v>85</v>
+      </c>
+      <c r="E1" s="1" t="s">
+        <v>92</v>
+      </c>
+      <c r="F1" s="1" t="s">
+        <v>93</v>
+      </c>
+      <c r="G1" s="1" t="s">
+        <v>94</v>
+      </c>
+      <c r="H1" s="1" t="s">
+        <v>95</v>
       </c>
       <c r="I1" s="1" t="s">
-        <v>44</v>
-      </c>
+        <v>96</v>
+      </c>
+      <c r="J1" s="1" t="s">
+        <v>97</v>
+      </c>
+      <c r="K1" s="1" t="s">
+        <v>98</v>
+      </c>
+      <c r="L1" s="1" t="s">
+        <v>99</v>
+      </c>
+      <c r="M1" s="1" t="s">
+        <v>100</v>
+      </c>
+      <c r="N1" s="1" t="s">
+        <v>101</v>
+      </c>
+      <c r="O1" s="1"/>
+      <c r="P1" s="1"/>
+      <c r="Q1" s="1"/>
+      <c r="R1" s="1"/>
+      <c r="S1" s="1"/>
     </row>
-    <row r="2" spans="1:9" x14ac:dyDescent="0.25">
-      <c r="A2" s="18" t="s">
-        <v>80</v>
-      </c>
-      <c r="B2" s="18" t="s">
+    <row r="2" spans="1:19" customFormat="1" x14ac:dyDescent="0.25">
+      <c r="A2" s="2" t="s">
         <v>2</v>
       </c>
-      <c r="C2" s="18" t="s">
-        <v>14</v>
-      </c>
-      <c r="D2" s="18" t="s">
-        <v>77</v>
-      </c>
-      <c r="E2" s="18" t="s">
-        <v>25</v>
-      </c>
-      <c r="F2" s="18" t="s">
-        <v>78</v>
-      </c>
-      <c r="G2" s="18" t="s">
-        <v>79</v>
-      </c>
-      <c r="H2" s="18"/>
-      <c r="I2" s="19" t="s">
-        <v>67</v>
+      <c r="B2" t="s">
+        <v>102</v>
+      </c>
+      <c r="C2" s="22" t="s">
+        <v>88</v>
+      </c>
+      <c r="D2" s="23" t="s">
+        <v>91</v>
+      </c>
+      <c r="E2" t="s">
+        <v>103</v>
+      </c>
+      <c r="F2" t="s">
+        <v>104</v>
+      </c>
+      <c r="G2" t="s">
+        <v>105</v>
+      </c>
+      <c r="H2" t="s">
+        <v>106</v>
+      </c>
+      <c r="I2" s="22" t="s">
+        <v>107</v>
+      </c>
+      <c r="J2" s="22" t="s">
+        <v>107</v>
+      </c>
+      <c r="K2" s="22" t="s">
+        <v>108</v>
+      </c>
+      <c r="L2" s="22" t="s">
+        <v>109</v>
+      </c>
+      <c r="M2" s="24" t="s">
+        <v>110</v>
+      </c>
+      <c r="N2" s="22" t="s">
+        <v>111</v>
       </c>
     </row>
   </sheetData>

</xml_diff>